<commit_message>
Added interval support, fixed skipping files
</commit_message>
<xml_diff>
--- a/tests/configuration_files/data/column-mappings.xlsx
+++ b/tests/configuration_files/data/column-mappings.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF63BDD-A112-4BE3-B7D4-0C330EDF1EB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25CF1DE-5F0B-411E-8DF1-185B142EA717}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="0" windowWidth="12312" windowHeight="4848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5616" yWindow="0" windowWidth="12312" windowHeight="4848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Code</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>table1</t>
+  </si>
+  <si>
+    <t>INTERVAL</t>
+  </si>
+  <si>
+    <t>SLA</t>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,6 +550,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
     </row>

</xml_diff>